<commit_message>
printing out 3d co-ordinates
</commit_message>
<xml_diff>
--- a/assignment3/q2/cv_3.xlsx
+++ b/assignment3/q2/cv_3.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>x</t>
   </si>
@@ -34,6 +35,9 @@
   </si>
   <si>
     <t>z'</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -80,10 +84,13 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -854,373 +861,638 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
+      <c r="A1" s="3">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
         <f>PRODUCT(7,9.6)</f>
         <v>67.200000000000003</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
+    <row r="3">
+      <c r="A3" s="3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
         <f>PRODUCT(9.6,11)</f>
         <v>105.59999999999999</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
+    <row r="4">
+      <c r="A4" s="3">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
         <f>PRODUCT(2,32)</f>
         <v>64</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3">
         <f>PRODUCT(5,32)</f>
         <v>160</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
         <f>16+PRODUCT(32,2)</f>
         <v>80</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
         <f>16+PRODUCT(6,32)</f>
         <v>208</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <f>PRODUCT(4,9.6)</f>
+        <v>38.399999999999999</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <f t="shared" ref="C9:C10" si="0">PRODUCT(4,9.6)</f>
-        <v>38.399999999999999</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
+      <c r="A9" s="3">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3">
         <f>16+PRODUCT(3,32)</f>
         <v>112</v>
       </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
+      <c r="C9" s="3">
+        <f>PRODUCT(4,9.6)</f>
         <v>38.399999999999999</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
+    <row r="10">
+      <c r="A10" s="3">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3">
         <f>16+PRODUCT(2,32)</f>
         <v>80</v>
       </c>
-      <c r="C11">
-        <f t="shared" ref="C11:C12" si="1">PRODUCT(8,9.6)</f>
+      <c r="C10" s="3">
+        <f>PRODUCT(8,9.6)</f>
         <v>76.799999999999997</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
+    <row r="11">
+      <c r="A11" s="3">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3">
         <f>16+PRODUCT(5,32)</f>
         <v>176</v>
       </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
+      <c r="C11" s="3">
+        <f>PRODUCT(8,9.6)</f>
         <v>76.799999999999997</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13">
+    <row r="12">
+      <c r="A12" s="3">
+        <v>0</v>
+      </c>
+      <c r="B12" s="3">
         <f>PRODUCT(1,32)</f>
         <v>32</v>
       </c>
-      <c r="C13">
-        <f t="shared" ref="C13:C15" si="2">PRODUCT(11,9.6)</f>
+      <c r="C12" s="3">
+        <f>PRODUCT(11,9.6)</f>
         <v>105.59999999999999</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
+    <row r="13">
+      <c r="A13" s="3">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3">
         <f>PRODUCT(3,32)</f>
         <v>96</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="2"/>
+      <c r="C13" s="3">
+        <f>PRODUCT(11,9.6)</f>
         <v>105.59999999999999</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15">
+    <row r="14">
+      <c r="A14" s="3">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3">
         <f>PRODUCT(5,32)</f>
         <v>160</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="2"/>
+      <c r="C14" s="3">
+        <f>PRODUCT(11,9.6)</f>
         <v>105.59999999999999</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
+    <row r="15">
+      <c r="A15" s="3">
+        <v>0</v>
+      </c>
+      <c r="B15" s="3">
         <f>16+PRODUCT(1,32)</f>
         <v>48</v>
       </c>
-      <c r="C16">
-        <f t="shared" ref="C16:C18" si="3">PRODUCT(9.6,2)</f>
+      <c r="C15" s="3">
+        <f>PRODUCT(9.6,2)</f>
         <v>19.199999999999999</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
+    <row r="16">
+      <c r="A16" s="3">
+        <v>0</v>
+      </c>
+      <c r="B16" s="3">
         <f>16+PRODUCT(3,32)</f>
         <v>112</v>
       </c>
-      <c r="C17" s="3">
-        <f t="shared" si="3"/>
+      <c r="C16" s="3">
+        <f>PRODUCT(9.6,2)</f>
         <v>19.199999999999999</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18">
+    <row r="17">
+      <c r="A17" s="3">
+        <v>0</v>
+      </c>
+      <c r="B17" s="3">
         <f>16+PRODUCT(5,32)</f>
         <v>176</v>
       </c>
-      <c r="C18" s="3">
-        <f t="shared" si="3"/>
+      <c r="C17" s="3">
+        <f>PRODUCT(9.6,2)</f>
         <v>19.199999999999999</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19">
+    <row r="18">
+      <c r="A18" s="3">
         <f>16+32</f>
         <v>48</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20">
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3">
         <f>16+PRODUCT(3,32)</f>
         <v>112</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21">
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3">
         <f>16+PRODUCT(5,32)</f>
         <v>176</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22">
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3">
         <f>16+PRODUCT(7,32)</f>
         <v>240</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23">
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3">
         <f>PRODUCT(2,32)</f>
         <v>64</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <f t="shared" ref="C23:C25" si="4">PRODUCT(6,9.6)</f>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3">
+        <f>PRODUCT(6,9.6)</f>
         <v>57.599999999999994</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24">
+    <row r="23">
+      <c r="A23" s="3">
         <f>PRODUCT(4,32)</f>
         <v>128</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="4"/>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3">
+        <f>PRODUCT(6,9.6)</f>
         <v>57.599999999999994</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25">
+    <row r="24">
+      <c r="A24" s="3">
         <f>PRODUCT(6,32)</f>
         <v>192</v>
       </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="4"/>
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3">
+        <f>PRODUCT(6,9.6)</f>
         <v>57.599999999999994</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26">
+    <row r="25">
+      <c r="A25" s="3">
         <f>16+PRODUCT(3,32)</f>
         <v>112</v>
       </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <f t="shared" ref="C26:C29" si="5">PRODUCT(13,9.6)</f>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <f>PRODUCT(13,9.6)</f>
         <v>124.8</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27">
+    <row r="26">
+      <c r="A26" s="3">
         <f>16+PRODUCT(6,32)</f>
         <v>208</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="5"/>
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3">
+        <f>PRODUCT(13,9.6)</f>
         <v>124.8</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28">
-        <v>0</v>
-      </c>
-      <c r="B28">
+    <row r="27">
+      <c r="A27" s="3">
+        <v>0</v>
+      </c>
+      <c r="B27" s="3">
         <f>PRODUCT(3,32)</f>
         <v>96</v>
       </c>
-      <c r="C28">
-        <f t="shared" si="5"/>
+      <c r="C27" s="3">
+        <f>PRODUCT(13,9.6)</f>
         <v>124.8</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29">
-        <v>0</v>
-      </c>
-      <c r="B29">
+    <row r="28">
+      <c r="A28" s="3">
+        <v>0</v>
+      </c>
+      <c r="B28" s="3">
         <f>PRODUCT(6,32)</f>
         <v>192</v>
       </c>
-      <c r="C29">
-        <f t="shared" si="5"/>
+      <c r="C28" s="3">
+        <f>PRODUCT(13,9.6)</f>
         <v>124.8</v>
       </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3">
+        <v>0</v>
+      </c>
+      <c r="B29" s="3">
+        <f>PRODUCT(32,6)</f>
+        <v>192</v>
+      </c>
+      <c r="C29" s="3">
+        <f>PRODUCT(9.6,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3">
+        <v>0</v>
+      </c>
+      <c r="B30" s="3">
+        <f>PRODUCT(32,6)</f>
+        <v>192</v>
+      </c>
+      <c r="C30" s="3">
+        <f>PRODUCT(9.6,2)</f>
+        <v>19.199999999999999</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4">
+        <v>0</v>
+      </c>
+      <c r="B31" s="3">
+        <f>PRODUCT(32,6)</f>
+        <v>192</v>
+      </c>
+      <c r="C31" s="3">
+        <f>PRODUCT(9.6,4)</f>
+        <v>38.399999999999999</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4">
+        <v>0</v>
+      </c>
+      <c r="B32" s="3">
+        <f>PRODUCT(32,6)</f>
+        <v>192</v>
+      </c>
+      <c r="C32" s="3">
+        <f>PRODUCT(9.6,6)</f>
+        <v>57.599999999999994</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="4">
+        <v>0</v>
+      </c>
+      <c r="B33" s="3">
+        <f>PRODUCT(32,6)</f>
+        <v>192</v>
+      </c>
+      <c r="C33" s="3">
+        <f>PRODUCT(9.6,8)</f>
+        <v>76.799999999999997</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4">
+        <v>0</v>
+      </c>
+      <c r="B34" s="3">
+        <f>PRODUCT(32,6)</f>
+        <v>192</v>
+      </c>
+      <c r="C34" s="3">
+        <f>PRODUCT(9.6,10)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4">
+        <v>0</v>
+      </c>
+      <c r="B35" s="3">
+        <f>PRODUCT(32,6)</f>
+        <v>192</v>
+      </c>
+      <c r="C35" s="3">
+        <f>PRODUCT(9.6,13)</f>
+        <v>124.8</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4">
+        <v>0</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3">
+        <f>PRODUCT(9.6,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4">
+        <v>0</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3">
+        <f>PRODUCT(9.6,2)</f>
+        <v>19.199999999999999</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4">
+        <v>0</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3">
+        <f>PRODUCT(9.6,4)</f>
+        <v>38.399999999999999</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4">
+        <v>0</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3">
+        <f>PRODUCT(9.6,6)</f>
+        <v>57.599999999999994</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4">
+        <v>0</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3">
+        <f>PRODUCT(9.6,8)</f>
+        <v>76.799999999999997</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="4">
+        <v>0</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3">
+        <f>PRODUCT(9.6,10)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4">
+        <v>0</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3">
+        <f>PRODUCT(9.6,13)</f>
+        <v>124.8</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4">
+        <f>PRODUCT(7,32)+16</f>
+        <v>240</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3">
+        <f>PRODUCT(9.6,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4">
+        <f>PRODUCT(7,32)+16</f>
+        <v>240</v>
+      </c>
+      <c r="B44" s="3">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3">
+        <f>PRODUCT(9.6,2)</f>
+        <v>19.199999999999999</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4">
+        <f>PRODUCT(7,32)+16</f>
+        <v>240</v>
+      </c>
+      <c r="B45" s="3">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3">
+        <f>PRODUCT(9.6,4)</f>
+        <v>38.399999999999999</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4">
+        <f>PRODUCT(7,32)+16</f>
+        <v>240</v>
+      </c>
+      <c r="B46" s="3">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3">
+        <f>PRODUCT(9.6,6)</f>
+        <v>57.599999999999994</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4">
+        <f>PRODUCT(7,32)+16</f>
+        <v>240</v>
+      </c>
+      <c r="B47" s="3">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3">
+        <f>PRODUCT(9.6,8)</f>
+        <v>76.799999999999997</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4">
+        <f>PRODUCT(7,32)+16</f>
+        <v>240</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0</v>
+      </c>
+      <c r="C48" s="3">
+        <f>PRODUCT(9.6,10)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4">
+        <f>PRODUCT(7,32)+16</f>
+        <v>240</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0</v>
+      </c>
+      <c r="C49" s="3">
+        <f>PRODUCT(9.6,13)</f>
+        <v>124.8</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="5"/>
+      <c r="B50" s="6"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="5">
+        <v>2447</v>
+      </c>
+      <c r="B51" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -1239,173 +1511,366 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" ht="14.25"/>
-    <row r="2" ht="14.25">
-      <c r="A2" s="4">
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>PRODUCT(7,9.6)</f>
+        <v>67.200000000000003</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f>PRODUCT(9.6,11)</f>
+        <v>105.59999999999999</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <f>PRODUCT(2,32)</f>
+        <v>64</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <f>PRODUCT(5,32)</f>
+        <v>160</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <f>16+PRODUCT(32,2)</f>
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <f>16+PRODUCT(6,32)</f>
+        <v>208</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:C10" si="0">PRODUCT(4,9.6)</f>
+        <v>38.399999999999999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <f>16+PRODUCT(3,32)</f>
+        <v>112</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>38.399999999999999</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <f>16+PRODUCT(2,32)</f>
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:C12" si="1">PRODUCT(8,9.6)</f>
+        <v>76.799999999999997</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <f>16+PRODUCT(5,32)</f>
+        <v>176</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>76.799999999999997</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <f>PRODUCT(1,32)</f>
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:C15" si="2">PRODUCT(11,9.6)</f>
+        <v>105.59999999999999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <f>PRODUCT(3,32)</f>
+        <v>96</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>105.59999999999999</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <f>PRODUCT(5,32)</f>
+        <v>160</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>105.59999999999999</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <f>16+PRODUCT(1,32)</f>
+        <v>48</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C18" si="3">PRODUCT(9.6,2)</f>
+        <v>19.199999999999999</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <f>16+PRODUCT(3,32)</f>
+        <v>112</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="3"/>
+        <v>19.199999999999999</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <f>16+PRODUCT(5,32)</f>
+        <v>176</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="3"/>
+        <v>19.199999999999999</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <f>16+32</f>
+        <v>48</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <f>16+PRODUCT(3,32)</f>
+        <v>112</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <f>16+PRODUCT(5,32)</f>
+        <v>176</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <f>16+PRODUCT(7,32)</f>
         <v>240</v>
       </c>
-      <c r="B2" s="5">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="4">
-        <v>242</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="4">
-        <v>240</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1178</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="4">
-        <v>242</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6" s="4">
-        <v>245</v>
-      </c>
-      <c r="B6" s="5">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25">
-      <c r="A7" s="4">
-        <v>245</v>
-      </c>
-      <c r="B7" s="5">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25">
-      <c r="A8" s="4">
-        <v>250</v>
-      </c>
-      <c r="B8" s="5">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="4">
-        <v>988</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="4">
-        <v>991</v>
-      </c>
-      <c r="B10" s="5">
-        <v>1623</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25">
-      <c r="A11" s="4">
-        <v>988</v>
-      </c>
-      <c r="B11" s="5">
-        <v>1471</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25">
-      <c r="A12" s="4">
-        <v>991</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25">
-      <c r="A13" s="4">
-        <v>993</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1180</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25">
-      <c r="A14" s="4">
-        <v>998</v>
-      </c>
-      <c r="B14" s="5">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="15" ht="14.25">
-      <c r="A15" s="4">
-        <v>998</v>
-      </c>
-      <c r="B15" s="5">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25">
-      <c r="A16" s="4">
-        <v>2424</v>
-      </c>
-      <c r="B16" s="5">
-        <v>1506</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25">
-      <c r="A17" s="4">
-        <v>2421</v>
-      </c>
-      <c r="B17" s="5">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25">
-      <c r="A18" s="4">
-        <v>2424</v>
-      </c>
-      <c r="B18" s="5">
-        <v>1236</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25">
-      <c r="A19" s="4">
-        <v>2434</v>
-      </c>
-      <c r="B19" s="5">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25">
-      <c r="A20" s="4">
-        <v>2439</v>
-      </c>
-      <c r="B20" s="5">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25">
-      <c r="A21" s="4">
-        <v>2439</v>
-      </c>
-      <c r="B21" s="5">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25">
-      <c r="A22" s="4">
-        <v>2447</v>
-      </c>
-      <c r="B22" s="5">
-        <v>625</v>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <f>PRODUCT(2,32)</f>
+        <v>64</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:C25" si="4">PRODUCT(6,9.6)</f>
+        <v>57.599999999999994</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <f>PRODUCT(4,32)</f>
+        <v>128</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="4"/>
+        <v>57.599999999999994</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <f>PRODUCT(6,32)</f>
+        <v>192</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="4"/>
+        <v>57.599999999999994</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <f>16+PRODUCT(3,32)</f>
+        <v>112</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:C29" si="5">PRODUCT(13,9.6)</f>
+        <v>124.8</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <f>16+PRODUCT(6,32)</f>
+        <v>208</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="5"/>
+        <v>124.8</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <f>PRODUCT(3,32)</f>
+        <v>96</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="5"/>
+        <v>124.8</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <f>PRODUCT(6,32)</f>
+        <v>192</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="5"/>
+        <v>124.8</v>
       </c>
     </row>
   </sheetData>
@@ -1423,14 +1888,218 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="5">
+        <v>240</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="5">
+        <v>242</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="5">
+        <v>240</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="5">
+        <v>242</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="5">
+        <v>245</v>
+      </c>
+      <c r="B6" s="6">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="5">
+        <v>245</v>
+      </c>
+      <c r="B7" s="6">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="5">
+        <v>250</v>
+      </c>
+      <c r="B8" s="6">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="5">
+        <v>988</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="5">
+        <v>991</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="5">
+        <v>988</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="5">
+        <v>991</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="5">
+        <v>993</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="5">
+        <v>998</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="5">
+        <v>998</v>
+      </c>
+      <c r="B15" s="6">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="5">
+        <v>2424</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="5">
+        <v>2421</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="5">
+        <v>2424</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="5">
+        <v>2434</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="5">
+        <v>2439</v>
+      </c>
+      <c r="B20" s="6">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="5">
+        <v>2439</v>
+      </c>
+      <c r="B21" s="6">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="5">
+        <v>2447</v>
+      </c>
+      <c r="B22" s="6">
+        <v>625</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <f>PRODUCT(32,6)</f>
+        <f t="shared" ref="B2:B8" si="6">PRODUCT(32,6)</f>
         <v>192</v>
       </c>
       <c r="C2">
@@ -1443,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <f>PRODUCT(32,6)</f>
+        <f t="shared" si="6"/>
         <v>192</v>
       </c>
       <c r="C3">
@@ -1456,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <f>PRODUCT(32,6)</f>
+        <f t="shared" si="6"/>
         <v>192</v>
       </c>
       <c r="C4">
@@ -1469,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <f>PRODUCT(32,6)</f>
+        <f t="shared" si="6"/>
         <v>192</v>
       </c>
       <c r="C5">
@@ -1482,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <f>PRODUCT(32,6)</f>
+        <f t="shared" si="6"/>
         <v>192</v>
       </c>
       <c r="C6">
@@ -1495,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <f>PRODUCT(32,6)</f>
+        <f t="shared" si="6"/>
         <v>192</v>
       </c>
       <c r="C7">
@@ -1508,7 +2177,7 @@
         <v>0</v>
       </c>
       <c r="B8">
-        <f>PRODUCT(32,6)</f>
+        <f t="shared" si="6"/>
         <v>192</v>
       </c>
       <c r="C8">
@@ -1602,7 +2271,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <f>PRODUCT(7,32)+16</f>
+        <f t="shared" ref="A16:A22" si="7">PRODUCT(7,32)+16</f>
         <v>240</v>
       </c>
       <c r="B16">
@@ -1615,7 +2284,7 @@
     </row>
     <row r="17">
       <c r="A17" s="3">
-        <f>PRODUCT(7,32)+16</f>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="B17">
@@ -1628,7 +2297,7 @@
     </row>
     <row r="18">
       <c r="A18" s="3">
-        <f>PRODUCT(7,32)+16</f>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="B18">
@@ -1641,7 +2310,7 @@
     </row>
     <row r="19">
       <c r="A19" s="3">
-        <f>PRODUCT(7,32)+16</f>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="B19">
@@ -1654,7 +2323,7 @@
     </row>
     <row r="20">
       <c r="A20" s="3">
-        <f>PRODUCT(7,32)+16</f>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="B20">
@@ -1667,7 +2336,7 @@
     </row>
     <row r="21">
       <c r="A21" s="3">
-        <f>PRODUCT(7,32)+16</f>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="B21">
@@ -1680,7 +2349,7 @@
     </row>
     <row r="22">
       <c r="A22" s="3">
-        <f>PRODUCT(7,32)+16</f>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="B22">

</xml_diff>